<commit_message>
adding controllers, index and service mvc layer full
</commit_message>
<xml_diff>
--- a/TCER MVC.xlsx
+++ b/TCER MVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ash_7\Desktop\DI001\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E61F88-28C1-40C0-A449-ADC2537A961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A636B40-217E-45D4-846E-2488A21F31B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-13290" windowWidth="17280" windowHeight="9420" xr2:uid="{C202E298-38B0-4EC8-9EEE-968DC7631DB1}"/>
+    <workbookView xWindow="4650" yWindow="-13725" windowWidth="17280" windowHeight="9420" xr2:uid="{C202E298-38B0-4EC8-9EEE-968DC7631DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>TCER for MVC Servvice</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>List of all books</t>
-  </si>
-  <si>
-    <t>GBL- neg</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
 </sst>
 </file>
@@ -409,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF16D9C0-A61B-4FD9-84C5-6521D64BE1AF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,22 +443,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>